<commit_message>
Create more samples for the time multiplier (follow general load pattern)
</commit_message>
<xml_diff>
--- a/Pyomo/MILP_v1/Input_Files/InputData34.xlsx
+++ b/Pyomo/MILP_v1/Input_Files/InputData34.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filip Forro\PycharmProjects\MasterThesis\Pyomo\MILP_v1\Input_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E950F9-B177-4037-8BC8-8C11F68C9AA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5064D60C-4D62-470D-8F85-CA8152629F7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="890" activeTab="12" xr2:uid="{C29AC206-A880-42C7-97CB-0C3D79BA6B73}"/>
   </bookViews>
@@ -4134,7 +4134,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4169,7 +4169,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.8</v>
+        <v>0.78</v>
       </c>
       <c r="C3">
         <v>40</v>
@@ -4180,7 +4180,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>0.72</v>
       </c>
       <c r="C4">
         <v>40</v>
@@ -4191,7 +4191,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.8</v>
+        <v>0.71</v>
       </c>
       <c r="C5">
         <v>45</v>
@@ -4202,7 +4202,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.8</v>
+        <v>0.76</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -4213,7 +4213,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.8</v>
+        <v>0.97</v>
       </c>
       <c r="C7">
         <v>55</v>
@@ -4224,7 +4224,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C8">
         <v>55</v>
@@ -4235,7 +4235,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="C9">
         <v>55</v>
@@ -4246,7 +4246,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -4257,7 +4257,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0.91</v>
       </c>
       <c r="C11">
         <v>50</v>
@@ -4268,7 +4268,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0.86</v>
       </c>
       <c r="C12">
         <v>50</v>
@@ -4279,7 +4279,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0.82</v>
       </c>
       <c r="C13">
         <v>50</v>
@@ -4290,7 +4290,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C14">
         <v>50</v>
@@ -4301,7 +4301,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0.94</v>
       </c>
       <c r="C15">
         <v>50</v>
@@ -4312,7 +4312,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="C16">
         <v>50</v>
@@ -4323,7 +4323,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>1.03</v>
       </c>
       <c r="C17">
         <v>50</v>
@@ -4334,7 +4334,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="C18">
         <v>50</v>
@@ -4345,7 +4345,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>1.2</v>
+        <v>1.25</v>
       </c>
       <c r="C19">
         <v>60</v>
@@ -4356,7 +4356,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>1.2</v>
+        <v>1.23</v>
       </c>
       <c r="C20">
         <v>60</v>
@@ -4367,7 +4367,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>1.2</v>
+        <v>1.18</v>
       </c>
       <c r="C21">
         <v>60</v>
@@ -4378,7 +4378,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>1.2</v>
+        <v>1.03</v>
       </c>
       <c r="C22">
         <v>60</v>
@@ -4389,7 +4389,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>1.2</v>
+        <v>0.99</v>
       </c>
       <c r="C23">
         <v>60</v>
@@ -4400,7 +4400,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>1.2</v>
+        <v>0.92</v>
       </c>
       <c r="C24">
         <v>60</v>
@@ -4411,7 +4411,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>1.2</v>
+        <v>0.84</v>
       </c>
       <c r="C25">
         <v>60</v>

</xml_diff>

<commit_message>
Added inflexible load to 20% of maximum load and changed the maximum allowable block consumption to 1/4 of the maximum load. Now, the block sizes are independent of time and approximated load but are based on maximum consumption so user is not limited to how much he can consume. Pd_imt is set to 1/4 of the maximum allowable consumption which is constrained by the physical connection capacity (AGG(Pd)).
</commit_message>
<xml_diff>
--- a/Pyomo/MILP_v1/Input_Files/InputData34.xlsx
+++ b/Pyomo/MILP_v1/Input_Files/InputData34.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filip Forro\PycharmProjects\MasterThesis\Pyomo\MILP_v1\Input_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5064D60C-4D62-470D-8F85-CA8152629F7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7781B3-4D14-4255-9526-CB26C67590E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="890" activeTab="12" xr2:uid="{C29AC206-A880-42C7-97CB-0C3D79BA6B73}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="890" activeTab="9" xr2:uid="{C29AC206-A880-42C7-97CB-0C3D79BA6B73}"/>
   </bookViews>
   <sheets>
     <sheet name="LineData" sheetId="3" r:id="rId1"/>
@@ -1569,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C358DC-12EF-4E1A-B9B4-66615C268D13}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4133,7 +4133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E9CC84-213D-4985-AA31-FE31D3539A2C}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>